<commit_message>
Final version after paper
</commit_message>
<xml_diff>
--- a/glass_fragments_procssed.xlsx
+++ b/glass_fragments_procssed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://biu365-my.sharepoint.com/personal/kaspiom_biu_ac_il/Documents/Projects/Police/Glass/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://biu365-my.sharepoint.com/personal/kaspiom_biu_ac_il/Documents/Projects/Police/Glass/GIT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="11_2D827874CA9A3ADFE0D129C4F5FEB68FB68FA7F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B129D69C-3B29-40A2-ADAA-6C5A614B019B}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="11_2D827874CA9A3ADFE0D129C4F5FEB68FB68FA7F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09D00B29-6F66-45AB-8A9A-734C5FCCEA26}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="unknown_irb_290821_surface" sheetId="8" r:id="rId8"/>
     <sheet name="unknown_irb_270921" sheetId="10" r:id="rId9"/>
     <sheet name="unknown_irb_290921_bulk" sheetId="11" r:id="rId10"/>
-    <sheet name="unknown_hu" sheetId="7" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId11"/>
+    <sheet name="unknown_hu" sheetId="7" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$D$1:$AD$381</definedName>
@@ -2309,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL789"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A756" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A778" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AL770" sqref="AL770:AV789"/>
     </sheetView>
   </sheetViews>
@@ -64494,8 +64495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -65105,6 +65106,18 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A488A202-686C-4A4A-826F-3498319D51C0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:BB11"/>
   <sheetViews>

</xml_diff>